<commit_message>
Split summarizing data into two slide decks.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA606 2022 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0EF78A-A23C-B44F-BA47-175600DAEFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE00F2D-C8DE-9C47-8C09-56E97A72188F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6180" yWindow="8340" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>Hu0-cNTcnuQ</t>
-  </si>
-  <si>
-    <t>02-Summarizing_Data</t>
   </si>
   <si>
     <t>mZwF_TLieQE</t>
@@ -289,6 +286,12 @@
 4 / 0 # Why is this Inf
 0 / 4
 ```</t>
+  </si>
+  <si>
+    <t>02-Summarizing_Data1</t>
+  </si>
+  <si>
+    <t>02-Summarizing_Data2</t>
   </si>
 </sst>
 </file>
@@ -674,7 +677,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,7 +783,7 @@
         <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -800,13 +803,13 @@
         <v>29</v>
       </c>
       <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="G5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>